<commit_message>
Created XGBoost for diff medicines
</commit_message>
<xml_diff>
--- a/outputs/forecast_DESWIN__TAB_8weeks_XGB.xlsx
+++ b/outputs/forecast_DESWIN__TAB_8weeks_XGB.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>59</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>59</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>59</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>59</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>59</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>59</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>59</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
XGB new and old prediction tried
</commit_message>
<xml_diff>
--- a/outputs/forecast_DESWIN__TAB_8weeks_XGB.xlsx
+++ b/outputs/forecast_DESWIN__TAB_8weeks_XGB.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,15 +436,10 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Medicine</t>
+          <t>Week</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Future_Week_Label</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Predicted_Quantity</t>
         </is>
@@ -453,121 +448,81 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DESWIN  TAB</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Future Week 1</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>30</v>
+          <t>2025-W43</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DESWIN  TAB</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Future Week 2</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>34</v>
+          <t>2025-W44</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DESWIN  TAB</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Future Week 3</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>34</v>
+          <t>2025-W45</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DESWIN  TAB</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Future Week 4</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>34</v>
+          <t>2025-W46</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DESWIN  TAB</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Future Week 5</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>34</v>
+          <t>2025-W47</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DESWIN  TAB</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Future Week 6</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>34</v>
+          <t>2025-W48</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DESWIN  TAB</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Future Week 7</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>35</v>
+          <t>2025-W49</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DESWIN  TAB</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Future Week 8</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>35</v>
+          <t>2025-W50</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>